<commit_message>
Updated valves_matrix_edited.xlsx with more information
</commit_message>
<xml_diff>
--- a/valves_matrix_edited.xlsx
+++ b/valves_matrix_edited.xlsx
@@ -83,55 +83,55 @@
     <t xml:space="preserve">timer_up_opening</t>
   </si>
   <si>
+    <t xml:space="preserve">error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signal_open_recieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">command_open_recieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open, start_timer_opening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPENING</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLOSING</t>
   </si>
   <si>
-    <t xml:space="preserve">signal_open_recieved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log_error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAULT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">command_open_recieved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error</t>
+    <t xml:space="preserve">reset_timer_closing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alert_error, log_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open, start_timer_opening, reset_timer_closing</t>
   </si>
   <si>
     <t xml:space="preserve">INIT</t>
   </si>
   <si>
+    <t xml:space="preserve">close, start_timer_closing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open, start_timer_opnening</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPEN</t>
   </si>
   <si>
-    <t xml:space="preserve">OPENING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reset_timer_closing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">close, start_timer_closing</t>
-  </si>
-  <si>
     <t xml:space="preserve">close, start_timer_closing, reset_timer_opening</t>
   </si>
   <si>
-    <t xml:space="preserve">alert_error, log_error</t>
-  </si>
-  <si>
     <t xml:space="preserve">reset_timer_opening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open, start_timer_opening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open, start_timer_opening, reset_timer_closing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open, start_timer_opnening</t>
   </si>
   <si>
     <t xml:space="preserve">POSSIBLE_ACTIONS</t>
@@ -339,16 +339,16 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
@@ -439,52 +439,52 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>12</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>14</v>
@@ -509,13 +509,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="C12" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>13</v>
@@ -523,13 +523,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>13</v>
@@ -537,66 +537,66 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="D15" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>12</v>
@@ -607,10 +607,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>12</v>
@@ -621,13 +621,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>13</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>12</v>
@@ -649,10 +649,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>12</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>12</v>
@@ -677,10 +677,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>12</v>
@@ -691,24 +691,24 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>12</v>
@@ -719,10 +719,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>12</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>12</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>12</v>
@@ -761,10 +761,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>12</v>
@@ -775,254 +775,254 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="D46" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,13 +1030,13 @@
         <v>24</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1112,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,7 +1120,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,7 +1128,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,7 +1194,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,7 +1218,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>